<commit_message>
mudanças no gerenciamento do projeto e roteiro de teste
</commit_message>
<xml_diff>
--- a/Desenvolvimento/4.Teste/Mais Dividendos - Roteiro de Testes.xlsx
+++ b/Desenvolvimento/4.Teste/Mais Dividendos - Roteiro de Testes.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\AGP\Desenvolvimento\4.Teste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEADA5B0-0CDE-4B88-9821-013F56B0292A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4230E63-CD3B-4FA8-AF57-8614E610791E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="913" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="913" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
     <sheet name="AUX" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="UC01" sheetId="3" r:id="rId3"/>
+    <sheet name="UC02" sheetId="6" r:id="rId4"/>
+    <sheet name="UC03" sheetId="5" r:id="rId5"/>
+    <sheet name="UC04" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="___xlfn_IFERROR">NA()</definedName>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>Mais Dividendos</t>
   </si>
@@ -70,6 +73,15 @@
     <t>UC01</t>
   </si>
   <si>
+    <t>UC02</t>
+  </si>
+  <si>
+    <t>UC03</t>
+  </si>
+  <si>
+    <t>UC05</t>
+  </si>
+  <si>
     <t>Totais</t>
   </si>
   <si>
@@ -128,13 +140,152 @@
   </si>
   <si>
     <t>Ver o preço da ação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC02 - Consultar agenda de dividendos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consultar agenda de dividendos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuário estar logado. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consultar informações sobre a agenda de dividendos selecionada  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código da ação </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informações limitadas exibidas corretamente  </t>
+  </si>
+  <si>
+    <r>
+      <t>Consultar informações com filtros</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Aplicar filtros de ações</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Filtragem de informações realizada com sucesso </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>UC03 – Login/Cadastro (autenticação/autorização)</t>
+  </si>
+  <si>
+    <t>Usuário estar logado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadastrar novos usuários com um email valido  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email valido e senha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autenticação do email e cadastro do usuario </t>
+  </si>
+  <si>
+    <r>
+      <t>Usuário cadastrado ter suas credenciais validadas e entrar na conta</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Email e senha validados e cadastrados </t>
+  </si>
+  <si>
+    <r>
+      <t>Acesso a conta</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">UC04 – Manter Carteiras de investimentos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manter Carteiras de investimentos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadastrar uma nova carteira </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome da carteira e descrição </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nova carteira criada e exibida na lista de carteiras </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editar uma carteira existente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome ou descrição atualizados </t>
+  </si>
+  <si>
+    <t>Atualização refletida na lista de carteiras </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excluir uma carteira </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identificação da carteira a ser excluída </t>
+  </si>
+  <si>
+    <t>Carteira removida da lista </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -318,6 +469,31 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="17">
@@ -418,7 +594,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -701,6 +877,115 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,7 +1007,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -814,23 +1099,84 @@
     <xf numFmtId="0" fontId="22" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="Bad" xfId="5" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Bom" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Calculation" xfId="2" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="2" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Célula de Verificação" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="4" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="4" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Neutra" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Note" xfId="8" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="8" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Porcentagem 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Ruim" xfId="5" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="11" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título 5" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Total" xfId="14" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="11" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1263,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.9"/>
@@ -1340,8 +1686,12 @@
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="20"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="17">
+        <v>2</v>
+      </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -1349,7 +1699,9 @@
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="20"/>
-      <c r="C7" s="16"/>
+      <c r="C7" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="D7" s="17"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -1358,7 +1710,9 @@
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="20"/>
-      <c r="C8" s="16"/>
+      <c r="C8" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="D8" s="17"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -1467,7 +1821,7 @@
     <row r="20" spans="2:12">
       <c r="B20" s="20"/>
       <c r="C20" s="18" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D20" s="18"/>
       <c r="F20" s="12"/>
@@ -1479,11 +1833,11 @@
       <c r="B21" s="20"/>
       <c r="C21" s="17">
         <f>COUNTA(C5:C19)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D21" s="17">
         <f>SUM(D5:D19)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F21" s="3">
         <f>SUM(F5:F19)</f>
@@ -1544,17 +1898,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1601,58 +1955,58 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1">
       <c r="A3" s="36" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
     </row>
     <row r="4" spans="1:23" ht="16.5" customHeight="1">
       <c r="A4" s="37" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="38"/>
       <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1">
       <c r="A5" s="27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="31" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="29" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1"/>
     <row r="8" spans="1:23" ht="15" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="16.5" customHeight="1">
@@ -1660,13 +2014,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -1710,4 +2064,489 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AFD457-8F94-4699-96DB-D49701289A4A}">
+  <dimension ref="A1:W10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="100.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1">
+      <c r="A1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:23" ht="18">
+      <c r="A2" s="35">
+        <v>2</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1">
+      <c r="A3" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1">
+      <c r="A4" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1">
+      <c r="A5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1"/>
+    <row r="8" spans="1:23" ht="15" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="57.75" customHeight="1">
+      <c r="A9" s="47">
+        <v>1</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" s="41" customFormat="1" ht="24" customHeight="1">
+      <c r="A10" s="39">
+        <v>2</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3434E8BD-80F4-4F11-B666-823EFD4FECFC}">
+  <dimension ref="A1:W10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="100.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1">
+      <c r="A1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:23" ht="18">
+      <c r="A2" s="35">
+        <v>2</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1">
+      <c r="A3" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1">
+      <c r="A4" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1">
+      <c r="A5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1"/>
+    <row r="8" spans="1:23" ht="15" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="28.5" customHeight="1">
+      <c r="A9" s="43">
+        <v>1</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" ht="35.25">
+      <c r="A10" s="39">
+        <v>2</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D143107-96EA-4070-9DCF-E3B2CFECF25F}">
+  <dimension ref="A1:W11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="B8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="100.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1">
+      <c r="A1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:23" ht="18">
+      <c r="A2" s="35">
+        <v>3</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1">
+      <c r="A3" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1">
+      <c r="A4" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1">
+      <c r="A5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1"/>
+    <row r="8" spans="1:23" ht="15" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="46.5" customHeight="1">
+      <c r="A9" s="43">
+        <v>1</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="53"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" ht="30" customHeight="1">
+      <c r="A10" s="56">
+        <v>2</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="54"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="49">
+        <v>3</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="54"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>